<commit_message>
como montar o tracker
</commit_message>
<xml_diff>
--- a/Docto-Paulo/Suporte-ThermoSafeSite.xlsx
+++ b/Docto-Paulo/Suporte-ThermoSafeSite.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11910" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tracker-local-locaweb" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="234">
   <si>
     <t>Opção A — com Docker (recomendado: 1 comando e tudo sobe)</t>
   </si>
@@ -1650,13 +1651,7 @@
     <t>http://localhost:8080</t>
   </si>
   <si>
-    <t>fazer teste do index.html</t>
-  </si>
-  <si>
     <t>http://localhost:8081</t>
-  </si>
-  <si>
-    <t>acessar phpMyAdmin</t>
   </si>
 </sst>
 </file>
@@ -1770,56 +1765,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1845,13 +1858,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
       <xdr:row>88</xdr:row>
-      <xdr:rowOff>45898</xdr:rowOff>
+      <xdr:rowOff>45899</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>108</xdr:row>
-      <xdr:rowOff>71971</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4781176</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1874,8 +1887,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="695325" y="16105048"/>
-          <a:ext cx="6076950" cy="3836073"/>
+          <a:off x="695325" y="19572149"/>
+          <a:ext cx="4695451" cy="2964002"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2150,290 +2163,290 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D449"/>
+  <dimension ref="B1:D317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A430" workbookViewId="0">
-      <selection activeCell="B449" sqref="B449"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="A124" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="60.5703125" customWidth="1"/>
+    <col min="2" max="2" width="73" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="31.5">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="2:2" ht="94.5">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="23.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:2">
-      <c r="B4" s="1"/>
+      <c r="B4" s="5"/>
     </row>
     <row r="5" spans="2:2">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:2">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:2">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:2">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:2">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:2">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:2">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:2">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:2">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="2:2">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="2:2" ht="23.25">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="2:2">
-      <c r="B17" s="1"/>
+      <c r="B17" s="5"/>
     </row>
     <row r="18" spans="2:2">
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="2:2">
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="2:2">
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:2">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:2">
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" spans="2:2">
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="24" spans="2:2">
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="25" spans="2:2">
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="26" spans="2:2">
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="27" spans="2:2">
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="28" spans="2:2">
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="29" spans="2:2">
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="30" spans="2:2">
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="31" spans="2:2">
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="32" spans="2:2">
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="33" spans="2:2">
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="34" spans="2:2">
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="35" spans="2:2">
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="36" spans="2:2">
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="37" spans="2:2">
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="38" spans="2:2">
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="39" spans="2:2">
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="40" spans="2:2">
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="41" spans="2:2">
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="42" spans="2:2">
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="43" spans="2:2">
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="44" spans="2:2">
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="45" spans="2:2">
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="46" spans="2:2">
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="47" spans="2:2">
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="48" spans="2:2">
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="50" spans="2:2">
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="7" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="51" spans="2:2">
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="52" spans="2:2">
-      <c r="B52" s="8" t="s">
+    <row r="52" spans="2:2" ht="45">
+      <c r="B52" s="7" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="53" spans="2:2">
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="8" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="54" spans="2:2">
-      <c r="B54" s="15" t="s">
+      <c r="B54" s="8" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="55" spans="2:2">
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="8" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="56" spans="2:2">
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="8" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="57" spans="2:2">
-      <c r="B57" s="15" t="s">
+      <c r="B57" s="8" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="58" spans="2:2">
-      <c r="B58" s="15" t="s">
+      <c r="B58" s="8" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="59" spans="2:2">
-      <c r="B59" s="8"/>
+      <c r="B59" s="7"/>
     </row>
     <row r="60" spans="2:2" ht="23.25">
       <c r="B60" s="9" t="s">
@@ -2485,12 +2498,12 @@
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="2:2">
+    <row r="70" spans="2:2" ht="30">
       <c r="B70" s="12" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="71" spans="2:2">
+    <row r="71" spans="2:2" ht="30">
       <c r="B71" s="12" t="s">
         <v>175</v>
       </c>
@@ -2510,13 +2523,13 @@
         <v>178</v>
       </c>
     </row>
-    <row r="75" spans="2:2">
-      <c r="B75" s="13" t="s">
+    <row r="75" spans="2:2" ht="30">
+      <c r="B75" s="11" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="76" spans="2:2">
-      <c r="B76" s="13" t="s">
+      <c r="B76" s="11" t="s">
         <v>180</v>
       </c>
     </row>
@@ -2531,7 +2544,7 @@
       </c>
     </row>
     <row r="79" spans="2:2">
-      <c r="B79" s="14" t="s">
+      <c r="B79" s="13" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2541,17 +2554,17 @@
       </c>
     </row>
     <row r="81" spans="2:2">
-      <c r="B81" s="13" t="s">
+      <c r="B81" s="11" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="82" spans="2:2">
-      <c r="B82" s="13" t="s">
+      <c r="B82" s="11" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="83" spans="2:2">
-      <c r="B83" s="13" t="s">
+      <c r="B83" s="11" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2565,950 +2578,1958 @@
         <v>188</v>
       </c>
     </row>
-    <row r="86" spans="2:2">
+    <row r="86" spans="2:2" ht="30">
       <c r="B86" s="11" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="87" spans="2:2">
+    <row r="87" spans="2:2" ht="30">
       <c r="B87" s="11" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="110" spans="2:2">
-      <c r="B110" t="s">
+    <row r="106" spans="2:2">
+      <c r="B106" s="14" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="111" spans="2:2" ht="18">
-      <c r="B111" s="16" t="s">
+    <row r="107" spans="2:2" ht="18">
+      <c r="B107" s="15" t="s">
         <v>199</v>
       </c>
     </row>
+    <row r="108" spans="2:2" ht="30">
+      <c r="B108" s="16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2">
+      <c r="B109" s="16" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2" ht="18">
+      <c r="B110" s="15" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2">
+      <c r="B111" s="14" t="s">
+        <v>203</v>
+      </c>
+    </row>
     <row r="112" spans="2:2">
-      <c r="B112" s="5" t="s">
-        <v>200</v>
+      <c r="B112" s="6" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="113" spans="2:2">
-      <c r="B113" s="5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="114" spans="2:2" ht="18">
-      <c r="B114" s="16" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="115" spans="2:2">
-      <c r="B115" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="116" spans="2:2">
-      <c r="B116" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="117" spans="2:2">
-      <c r="B117" t="s">
+      <c r="B113" s="14" t="s">
         <v>205</v>
       </c>
     </row>
+    <row r="114" spans="2:2">
+      <c r="B114" s="17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2" ht="18">
+      <c r="B117" s="15" t="s">
+        <v>206</v>
+      </c>
+    </row>
     <row r="118" spans="2:2">
-      <c r="B118" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="121" spans="2:2" ht="18">
-      <c r="B121" s="16" t="s">
-        <v>206</v>
+      <c r="B118" s="16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2">
+      <c r="B119" s="16" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2" ht="18">
+      <c r="B120" s="15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2">
+      <c r="B121" s="14" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="122" spans="2:2">
-      <c r="B122" s="5" t="s">
-        <v>207</v>
+      <c r="B122" s="6" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="123" spans="2:2">
-      <c r="B123" s="5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="124" spans="2:2" ht="18">
-      <c r="B124" s="16" t="s">
-        <v>209</v>
+      <c r="B123" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2">
+      <c r="B124" s="14" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="125" spans="2:2">
-      <c r="B125" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="126" spans="2:2">
-      <c r="B126" s="4" t="s">
-        <v>211</v>
+      <c r="B125" s="17" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="127" spans="2:2">
-      <c r="B127" s="4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="128" spans="2:2">
-      <c r="B128" t="s">
-        <v>213</v>
+      <c r="B127" s="17" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="129" spans="2:2">
       <c r="B129" s="17" t="s">
-        <v>216</v>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2" ht="45">
+      <c r="B130" s="14" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="131" spans="2:2">
-      <c r="B131" s="17" t="s">
+      <c r="B131" s="14" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2">
+      <c r="B132" s="14" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2">
+      <c r="B133" s="14" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2">
+      <c r="B134" s="17" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2" ht="45">
+      <c r="B135" s="14" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2">
+      <c r="B136" s="14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2" ht="30">
+      <c r="B137" s="14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2" ht="30">
+      <c r="B138" s="14" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2" ht="30">
+      <c r="B139" s="14" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2">
+      <c r="B140" s="14" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2" ht="23.25">
+      <c r="B141" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2">
+      <c r="B142" s="5"/>
+    </row>
+    <row r="143" spans="2:2">
+      <c r="B143" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2">
+      <c r="B144" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4">
+      <c r="B145" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4">
+      <c r="B146" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="148" spans="2:4" ht="23.25">
+      <c r="B148" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="149" spans="2:4">
+      <c r="B149" s="5"/>
+    </row>
+    <row r="150" spans="2:4">
+      <c r="B150" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4">
+      <c r="B151" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="152" spans="2:4">
+      <c r="B152" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="153" spans="2:4">
+      <c r="B153" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="154" spans="2:4">
+      <c r="B154" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4">
+      <c r="B155" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D155" s="2"/>
+    </row>
+    <row r="156" spans="2:4">
+      <c r="B156" s="5"/>
+    </row>
+    <row r="157" spans="2:4">
+      <c r="B157" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="158" spans="2:4">
+      <c r="B158" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D158" s="1"/>
+    </row>
+    <row r="159" spans="2:4">
+      <c r="B159" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="160" spans="2:4">
+      <c r="B160" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="161" spans="2:2">
+      <c r="B161" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="162" spans="2:2">
+      <c r="B162" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="165" spans="2:2" ht="23.25">
+      <c r="B165" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="166" spans="2:2">
+      <c r="B166" s="5"/>
+    </row>
+    <row r="167" spans="2:2">
+      <c r="B167" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="168" spans="2:2">
+      <c r="B168" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="169" spans="2:2">
+      <c r="B169" s="5"/>
+    </row>
+    <row r="170" spans="2:2">
+      <c r="B170" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="171" spans="2:2">
+      <c r="B171" s="5"/>
+    </row>
+    <row r="172" spans="2:2">
+      <c r="B172" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="173" spans="2:2">
+      <c r="B173" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="174" spans="2:2">
+      <c r="B174" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="175" spans="2:2">
+      <c r="B175" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="176" spans="2:2">
+      <c r="B176" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="177" spans="2:4">
+      <c r="B177" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="178" spans="2:4">
+      <c r="B178" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="179" spans="2:4">
+      <c r="B179" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D179" s="2"/>
+    </row>
+    <row r="180" spans="2:4">
+      <c r="B180" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="181" spans="2:4">
+      <c r="B181" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="182" spans="2:4">
+      <c r="B182" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="183" spans="2:4">
+      <c r="B183" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="184" spans="2:4">
+      <c r="B184" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="185" spans="2:4">
+      <c r="B185" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="186" spans="2:4">
+      <c r="B186" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="187" spans="2:4">
+      <c r="B187" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="188" spans="2:4">
+      <c r="B188" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="189" spans="2:4">
+      <c r="B189" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="190" spans="2:4">
+      <c r="B190" s="5"/>
+    </row>
+    <row r="191" spans="2:4">
+      <c r="B191" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="192" spans="2:4">
+      <c r="B192" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="193" spans="2:2">
+      <c r="B193" s="5"/>
+    </row>
+    <row r="194" spans="2:2">
+      <c r="B194" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="195" spans="2:2" ht="25.5">
+      <c r="B195" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="196" spans="2:2" ht="25.5">
+      <c r="B196" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="197" spans="2:2">
+      <c r="B197" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="198" spans="2:2">
+      <c r="B198" s="5"/>
+    </row>
+    <row r="199" spans="2:2">
+      <c r="B199" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="200" spans="2:2">
+      <c r="B200" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="201" spans="2:2">
+      <c r="B201" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="202" spans="2:2">
+      <c r="B202" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="203" spans="2:2">
+      <c r="B203" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="204" spans="2:2">
+      <c r="B204" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="205" spans="2:2">
+      <c r="B205" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="206" spans="2:2">
+      <c r="B206" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="207" spans="2:2">
+      <c r="B207" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="208" spans="2:2">
+      <c r="B208" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="209" spans="2:2">
+      <c r="B209" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="210" spans="2:2">
+      <c r="B210" s="5"/>
+    </row>
+    <row r="211" spans="2:2">
+      <c r="B211" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="214" spans="2:2" ht="23.25">
+      <c r="B214" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="215" spans="2:2">
+      <c r="B215" s="5"/>
+    </row>
+    <row r="216" spans="2:2">
+      <c r="B216" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="217" spans="2:2">
+      <c r="B217" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="218" spans="2:2">
+      <c r="B218" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="219" spans="2:2">
+      <c r="B219" s="5"/>
+    </row>
+    <row r="220" spans="2:2">
+      <c r="B220" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="221" spans="2:2">
+      <c r="B221" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="222" spans="2:2">
+      <c r="B222" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="223" spans="2:2">
+      <c r="B223" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="224" spans="2:2">
+      <c r="B224" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="225" spans="2:2">
+      <c r="B225" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="226" spans="2:2">
+      <c r="B226" s="5"/>
+    </row>
+    <row r="227" spans="2:2">
+      <c r="B227" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="228" spans="2:2">
+      <c r="B228" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="229" spans="2:2">
+      <c r="B229" s="5"/>
+    </row>
+    <row r="230" spans="2:2" ht="25.5">
+      <c r="B230" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="231" spans="2:2" ht="25.5">
+      <c r="B231" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="232" spans="2:2" ht="25.5">
+      <c r="B232" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="233" spans="2:2">
+      <c r="B233" s="5"/>
+    </row>
+    <row r="234" spans="2:2">
+      <c r="B234" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="235" spans="2:2">
+      <c r="B235" s="5"/>
+    </row>
+    <row r="236" spans="2:2">
+      <c r="B236" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="237" spans="2:2">
+      <c r="B237" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="238" spans="2:2">
+      <c r="B238" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="239" spans="2:2">
+      <c r="B239" s="5"/>
+    </row>
+    <row r="240" spans="2:2">
+      <c r="B240" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="241" spans="2:2">
+      <c r="B241" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="242" spans="2:2">
+      <c r="B242" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="243" spans="2:2">
+      <c r="B243" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="244" spans="2:2">
+      <c r="B244" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="245" spans="2:2">
+      <c r="B245" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="246" spans="2:2">
+      <c r="B246" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="247" spans="2:2">
+      <c r="B247" s="5"/>
+    </row>
+    <row r="248" spans="2:2">
+      <c r="B248" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="249" spans="2:2">
+      <c r="B249" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="250" spans="2:2">
+      <c r="B250" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="251" spans="2:2">
+      <c r="B251" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="252" spans="2:2">
+      <c r="B252" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="255" spans="2:2" ht="23.25">
+      <c r="B255" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="256" spans="2:2">
+      <c r="B256" s="5"/>
+    </row>
+    <row r="257" spans="2:2">
+      <c r="B257" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="258" spans="2:2">
+      <c r="B258" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="259" spans="2:2">
+      <c r="B259" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="260" spans="2:2">
+      <c r="B260" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="261" spans="2:2">
+      <c r="B261" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="262" spans="2:2">
+      <c r="B262" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="263" spans="2:2">
+      <c r="B263" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="264" spans="2:2">
+      <c r="B264" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="265" spans="2:2">
+      <c r="B265" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="266" spans="2:2">
+      <c r="B266" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="267" spans="2:2">
+      <c r="B267" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="268" spans="2:2">
+      <c r="B268" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="269" spans="2:2">
+      <c r="B269" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="270" spans="2:2">
+      <c r="B270" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="271" spans="2:2">
+      <c r="B271" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="272" spans="2:2">
+      <c r="B272" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="273" spans="2:2">
+      <c r="B273" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="274" spans="2:2">
+      <c r="B274" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="275" spans="2:2">
+      <c r="B275" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="276" spans="2:2">
+      <c r="B276" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="277" spans="2:2">
+      <c r="B277" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="278" spans="2:2">
+      <c r="B278" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="279" spans="2:2">
+      <c r="B279" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="280" spans="2:2">
+      <c r="B280" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="281" spans="2:2">
+      <c r="B281" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="282" spans="2:2">
+      <c r="B282" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="283" spans="2:2">
+      <c r="B283" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="284" spans="2:2">
+      <c r="B284" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="287" spans="2:2" ht="23.25">
+      <c r="B287" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="288" spans="2:2">
+      <c r="B288" s="16"/>
+    </row>
+    <row r="289" spans="2:2">
+      <c r="B289" s="16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="290" spans="2:2">
+      <c r="B290" s="16"/>
+    </row>
+    <row r="291" spans="2:2">
+      <c r="B291" s="16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="292" spans="2:2">
+      <c r="B292" s="5"/>
+    </row>
+    <row r="293" spans="2:2">
+      <c r="B293" s="6" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="133" spans="2:2">
-      <c r="B133" s="17" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="134" spans="2:2">
-      <c r="B134" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="135" spans="2:2">
-      <c r="B135" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="136" spans="2:2">
-      <c r="B136" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="137" spans="2:2">
-      <c r="B137" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="138" spans="2:2">
-      <c r="B138" s="17" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="139" spans="2:2">
-      <c r="B139" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="140" spans="2:2">
-      <c r="B140" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="141" spans="2:2">
-      <c r="B141" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="142" spans="2:2">
-      <c r="B142" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="143" spans="2:2">
-      <c r="B143" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="144" spans="2:2">
-      <c r="B144" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="145" spans="2:4" ht="23.25">
-      <c r="B145" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="146" spans="2:4">
-      <c r="B146" s="1"/>
-    </row>
-    <row r="147" spans="2:4">
-      <c r="B147" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="148" spans="2:4">
-      <c r="B148" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="149" spans="2:4">
-      <c r="B149" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="150" spans="2:4">
-      <c r="B150" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="152" spans="2:4" ht="23.25">
-      <c r="B152" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="153" spans="2:4">
-      <c r="B153" s="1"/>
-    </row>
-    <row r="154" spans="2:4">
-      <c r="B154" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="155" spans="2:4">
-      <c r="B155" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="156" spans="2:4">
-      <c r="B156" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="157" spans="2:4">
-      <c r="B157" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="158" spans="2:4">
-      <c r="B158" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="159" spans="2:4">
-      <c r="B159" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D159" s="5"/>
-    </row>
-    <row r="160" spans="2:4">
-      <c r="B160" s="1"/>
-    </row>
-    <row r="161" spans="2:4">
-      <c r="B161" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="162" spans="2:4">
-      <c r="B162" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D162" s="1"/>
-    </row>
-    <row r="163" spans="2:4">
-      <c r="B163" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="164" spans="2:4">
-      <c r="B164" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="165" spans="2:4">
-      <c r="B165" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="166" spans="2:4">
-      <c r="B166" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="198" spans="2:2" ht="23.25">
-      <c r="B198" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="199" spans="2:2">
-      <c r="B199" s="1"/>
-    </row>
-    <row r="200" spans="2:2">
-      <c r="B200" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="201" spans="2:2">
-      <c r="B201" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="202" spans="2:2">
-      <c r="B202" s="1"/>
-    </row>
-    <row r="203" spans="2:2">
-      <c r="B203" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="204" spans="2:2">
-      <c r="B204" s="1"/>
-    </row>
-    <row r="205" spans="2:2">
-      <c r="B205" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="206" spans="2:2">
-      <c r="B206" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="207" spans="2:2">
-      <c r="B207" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="208" spans="2:2">
-      <c r="B208" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="209" spans="2:4">
-      <c r="B209" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="210" spans="2:4">
-      <c r="B210" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="211" spans="2:4">
-      <c r="B211" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="212" spans="2:4">
-      <c r="B212" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D212" s="5"/>
-    </row>
-    <row r="213" spans="2:4">
-      <c r="B213" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="214" spans="2:4">
-      <c r="B214" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="215" spans="2:4">
-      <c r="B215" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="216" spans="2:4">
-      <c r="B216" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="217" spans="2:4">
-      <c r="B217" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="218" spans="2:4">
-      <c r="B218" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="219" spans="2:4">
-      <c r="B219" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="220" spans="2:4">
-      <c r="B220" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="221" spans="2:4">
-      <c r="B221" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="222" spans="2:4">
-      <c r="B222" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="223" spans="2:4">
-      <c r="B223" s="1"/>
-    </row>
-    <row r="224" spans="2:4">
-      <c r="B224" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="225" spans="2:2">
-      <c r="B225" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="226" spans="2:2">
-      <c r="B226" s="1"/>
-    </row>
-    <row r="227" spans="2:2">
-      <c r="B227" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="228" spans="2:2">
-      <c r="B228" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="229" spans="2:2">
-      <c r="B229" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="230" spans="2:2">
-      <c r="B230" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="231" spans="2:2">
-      <c r="B231" s="1"/>
-    </row>
-    <row r="232" spans="2:2">
-      <c r="B232" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="233" spans="2:2">
-      <c r="B233" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="234" spans="2:2">
-      <c r="B234" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="235" spans="2:2">
-      <c r="B235" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="236" spans="2:2">
-      <c r="B236" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="237" spans="2:2">
-      <c r="B237" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="238" spans="2:2">
-      <c r="B238" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="239" spans="2:2">
-      <c r="B239" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="240" spans="2:2">
-      <c r="B240" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="241" spans="2:2">
-      <c r="B241" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="242" spans="2:2">
-      <c r="B242" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="243" spans="2:2">
-      <c r="B243" s="1"/>
-    </row>
-    <row r="244" spans="2:2">
-      <c r="B244" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="279" spans="2:2" ht="23.25">
-      <c r="B279" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="280" spans="2:2">
-      <c r="B280" s="1"/>
-    </row>
-    <row r="281" spans="2:2">
-      <c r="B281" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="282" spans="2:2">
-      <c r="B282" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="283" spans="2:2">
-      <c r="B283" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="284" spans="2:2">
-      <c r="B284" s="1"/>
-    </row>
-    <row r="285" spans="2:2">
-      <c r="B285" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="286" spans="2:2">
-      <c r="B286" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="287" spans="2:2">
-      <c r="B287" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="288" spans="2:2">
-      <c r="B288" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="289" spans="2:2">
-      <c r="B289" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="290" spans="2:2">
-      <c r="B290" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="291" spans="2:2">
-      <c r="B291" s="1"/>
-    </row>
-    <row r="292" spans="2:2">
-      <c r="B292" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="293" spans="2:2">
-      <c r="B293" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
     <row r="294" spans="2:2">
-      <c r="B294" s="1"/>
+      <c r="B294" s="16"/>
     </row>
     <row r="295" spans="2:2">
-      <c r="B295" s="4" t="s">
-        <v>106</v>
+      <c r="B295" s="18" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="296" spans="2:2">
-      <c r="B296" s="4" t="s">
-        <v>107</v>
-      </c>
+      <c r="B296" s="16"/>
     </row>
     <row r="297" spans="2:2">
-      <c r="B297" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="298" spans="2:2">
-      <c r="B298" s="1"/>
-    </row>
-    <row r="299" spans="2:2">
-      <c r="B299" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="300" spans="2:2">
-      <c r="B300" s="1"/>
-    </row>
-    <row r="301" spans="2:2">
+      <c r="B297" s="18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="299" spans="2:2" ht="45">
+      <c r="B299" s="19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="301" spans="2:2" ht="23.25">
       <c r="B301" s="4" t="s">
-        <v>110</v>
+        <v>158</v>
       </c>
     </row>
     <row r="302" spans="2:2">
-      <c r="B302" s="4" t="s">
-        <v>111</v>
-      </c>
+      <c r="B302" s="16"/>
     </row>
     <row r="303" spans="2:2">
-      <c r="B303" s="4" t="s">
-        <v>112</v>
+      <c r="B303" s="16" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="304" spans="2:2">
-      <c r="B304" s="1"/>
+      <c r="B304" s="16"/>
     </row>
     <row r="305" spans="2:2">
-      <c r="B305" s="4" t="s">
-        <v>113</v>
+      <c r="B305" s="16" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="306" spans="2:2">
-      <c r="B306" s="4" t="s">
-        <v>114</v>
-      </c>
+      <c r="B306" s="16"/>
     </row>
     <row r="307" spans="2:2">
-      <c r="B307" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="308" spans="2:2">
-      <c r="B308" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="309" spans="2:2">
-      <c r="B309" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="310" spans="2:2">
-      <c r="B310" s="4" t="s">
-        <v>79</v>
+      <c r="B307" s="16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="309" spans="2:2" ht="30">
+      <c r="B309" s="14" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="311" spans="2:2">
-      <c r="B311" s="4" t="s">
-        <v>118</v>
+      <c r="B311" s="20" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="312" spans="2:2">
-      <c r="B312" s="1"/>
+      <c r="B312" s="20" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="313" spans="2:2">
-      <c r="B313" s="4" t="s">
-        <v>119</v>
+      <c r="B313" s="20" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="314" spans="2:2">
-      <c r="B314" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="315" spans="2:2">
-      <c r="B315" s="4" t="s">
-        <v>121</v>
+      <c r="B314" s="20" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="316" spans="2:2">
-      <c r="B316" s="4" t="s">
-        <v>122</v>
+      <c r="B316" s="21" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="317" spans="2:2">
-      <c r="B317" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="353" spans="2:2" ht="23.25">
-      <c r="B353" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="354" spans="2:2">
-      <c r="B354" s="1"/>
-    </row>
-    <row r="355" spans="2:2">
-      <c r="B355" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="356" spans="2:2">
-      <c r="B356" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="357" spans="2:2">
-      <c r="B357" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="358" spans="2:2">
-      <c r="B358" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="359" spans="2:2">
-      <c r="B359" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="360" spans="2:2">
-      <c r="B360" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="361" spans="2:2">
-      <c r="B361" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="362" spans="2:2">
-      <c r="B362" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="363" spans="2:2">
-      <c r="B363" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="364" spans="2:2">
-      <c r="B364" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="365" spans="2:2">
-      <c r="B365" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="366" spans="2:2">
-      <c r="B366" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="367" spans="2:2">
-      <c r="B367" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="368" spans="2:2">
-      <c r="B368" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="369" spans="2:2">
-      <c r="B369" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="370" spans="2:2">
-      <c r="B370" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="371" spans="2:2">
-      <c r="B371" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="372" spans="2:2">
-      <c r="B372" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="373" spans="2:2">
-      <c r="B373" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="374" spans="2:2">
-      <c r="B374" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="375" spans="2:2">
-      <c r="B375" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="376" spans="2:2">
-      <c r="B376" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="377" spans="2:2">
-      <c r="B377" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="378" spans="2:2">
-      <c r="B378" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="379" spans="2:2">
-      <c r="B379" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="380" spans="2:2">
-      <c r="B380" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="381" spans="2:2">
-      <c r="B381" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="382" spans="2:2">
-      <c r="B382" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="413" spans="2:2" ht="23.25">
-      <c r="B413" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="414" spans="2:2">
-      <c r="B414" s="5"/>
-    </row>
-    <row r="415" spans="2:2">
-      <c r="B415" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="416" spans="2:2">
-      <c r="B416" s="5"/>
-    </row>
-    <row r="417" spans="2:2">
-      <c r="B417" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="418" spans="2:2">
-      <c r="B418" s="1"/>
-    </row>
-    <row r="419" spans="2:2">
-      <c r="B419" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="420" spans="2:2">
-      <c r="B420" s="5"/>
-    </row>
-    <row r="421" spans="2:2">
-      <c r="B421" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="422" spans="2:2">
-      <c r="B422" s="5"/>
-    </row>
-    <row r="423" spans="2:2">
-      <c r="B423" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="425" spans="2:2">
-      <c r="B425" s="7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="430" spans="2:2" ht="23.25">
-      <c r="B430" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="431" spans="2:2">
-      <c r="B431" s="5"/>
-    </row>
-    <row r="432" spans="2:2">
-      <c r="B432" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="433" spans="2:3">
-      <c r="B433" s="5"/>
-    </row>
-    <row r="434" spans="2:3">
-      <c r="B434" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="435" spans="2:3">
-      <c r="B435" s="5"/>
-    </row>
-    <row r="436" spans="2:3">
-      <c r="B436" s="5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="438" spans="2:3">
-      <c r="B438" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="442" spans="2:3">
-      <c r="B442" s="18" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="443" spans="2:3">
-      <c r="B443" s="18" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="444" spans="2:3">
-      <c r="B444" s="18" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="445" spans="2:3">
-      <c r="B445" s="18" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="448" spans="2:3">
-      <c r="B448" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="C448" t="s">
+      <c r="B317" s="22" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="449" spans="2:3">
-      <c r="B449" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="C449" t="s">
-        <v>235</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B421" r:id="rId1" display="http://localhost:8080/"/>
-    <hyperlink ref="B423" r:id="rId2" display="http://localhost:8081/"/>
-    <hyperlink ref="B449" r:id="rId3"/>
-    <hyperlink ref="B448" r:id="rId4"/>
+    <hyperlink ref="B295" r:id="rId1" display="http://localhost:8080/"/>
+    <hyperlink ref="B297" r:id="rId2" display="http://localhost:8081/"/>
+    <hyperlink ref="B317" r:id="rId3"/>
+    <hyperlink ref="B316" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
   <drawing r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D226"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="73" style="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="94.5">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" ht="23.25">
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" s="5"/>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2">
+      <c r="B9" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" ht="23.25">
+      <c r="B16" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="5"/>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" ht="23.25">
+      <c r="B50" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="B51" s="5"/>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="B52" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4">
+      <c r="B53" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="B54" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4">
+      <c r="B55" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" ht="23.25">
+      <c r="B57" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4">
+      <c r="B58" s="5"/>
+    </row>
+    <row r="59" spans="2:4">
+      <c r="B59" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4">
+      <c r="B60" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4">
+      <c r="B61" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4">
+      <c r="B62" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4">
+      <c r="B63" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4">
+      <c r="B64" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="2:4">
+      <c r="B65" s="5"/>
+    </row>
+    <row r="66" spans="2:4">
+      <c r="B66" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4">
+      <c r="B67" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D67" s="1"/>
+    </row>
+    <row r="68" spans="2:4">
+      <c r="B68" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4">
+      <c r="B69" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4">
+      <c r="B70" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4">
+      <c r="B71" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" ht="23.25">
+      <c r="B74" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4">
+      <c r="B75" s="5"/>
+    </row>
+    <row r="76" spans="2:4">
+      <c r="B76" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4">
+      <c r="B77" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4">
+      <c r="B78" s="5"/>
+    </row>
+    <row r="79" spans="2:4">
+      <c r="B79" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4">
+      <c r="B80" s="5"/>
+    </row>
+    <row r="81" spans="2:4">
+      <c r="B81" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4">
+      <c r="B82" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4">
+      <c r="B83" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4">
+      <c r="B84" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4">
+      <c r="B85" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4">
+      <c r="B86" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4">
+      <c r="B87" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4">
+      <c r="B88" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="2:4">
+      <c r="B89" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4">
+      <c r="B90" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4">
+      <c r="B91" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4">
+      <c r="B92" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4">
+      <c r="B93" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4">
+      <c r="B94" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4">
+      <c r="B95" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4">
+      <c r="B96" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2">
+      <c r="B97" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2">
+      <c r="B98" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2">
+      <c r="B99" s="5"/>
+    </row>
+    <row r="100" spans="2:2">
+      <c r="B100" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2">
+      <c r="B101" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2">
+      <c r="B102" s="5"/>
+    </row>
+    <row r="103" spans="2:2">
+      <c r="B103" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" ht="25.5">
+      <c r="B104" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" ht="25.5">
+      <c r="B105" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2">
+      <c r="B106" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2">
+      <c r="B107" s="5"/>
+    </row>
+    <row r="108" spans="2:2">
+      <c r="B108" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2">
+      <c r="B109" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2">
+      <c r="B110" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2">
+      <c r="B111" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2">
+      <c r="B112" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2">
+      <c r="B113" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2">
+      <c r="B114" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2">
+      <c r="B115" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2">
+      <c r="B116" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2">
+      <c r="B117" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2">
+      <c r="B118" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2">
+      <c r="B119" s="5"/>
+    </row>
+    <row r="120" spans="2:2">
+      <c r="B120" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2" ht="23.25">
+      <c r="B123" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2">
+      <c r="B124" s="5"/>
+    </row>
+    <row r="125" spans="2:2">
+      <c r="B125" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2">
+      <c r="B126" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2">
+      <c r="B127" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2">
+      <c r="B128" s="5"/>
+    </row>
+    <row r="129" spans="2:2">
+      <c r="B129" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2">
+      <c r="B130" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2">
+      <c r="B131" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2">
+      <c r="B132" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2">
+      <c r="B133" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2">
+      <c r="B134" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2">
+      <c r="B135" s="5"/>
+    </row>
+    <row r="136" spans="2:2">
+      <c r="B136" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2">
+      <c r="B137" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2">
+      <c r="B138" s="5"/>
+    </row>
+    <row r="139" spans="2:2" ht="25.5">
+      <c r="B139" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2" ht="25.5">
+      <c r="B140" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2" ht="25.5">
+      <c r="B141" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2">
+      <c r="B142" s="5"/>
+    </row>
+    <row r="143" spans="2:2">
+      <c r="B143" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2">
+      <c r="B144" s="5"/>
+    </row>
+    <row r="145" spans="2:2">
+      <c r="B145" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2">
+      <c r="B146" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2">
+      <c r="B147" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2">
+      <c r="B148" s="5"/>
+    </row>
+    <row r="149" spans="2:2">
+      <c r="B149" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="150" spans="2:2">
+      <c r="B150" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="151" spans="2:2">
+      <c r="B151" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="152" spans="2:2">
+      <c r="B152" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="153" spans="2:2">
+      <c r="B153" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="154" spans="2:2">
+      <c r="B154" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="155" spans="2:2">
+      <c r="B155" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="156" spans="2:2">
+      <c r="B156" s="5"/>
+    </row>
+    <row r="157" spans="2:2">
+      <c r="B157" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="158" spans="2:2">
+      <c r="B158" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2">
+      <c r="B159" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="160" spans="2:2">
+      <c r="B160" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="161" spans="2:2">
+      <c r="B161" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="164" spans="2:2" ht="23.25">
+      <c r="B164" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="165" spans="2:2">
+      <c r="B165" s="5"/>
+    </row>
+    <row r="166" spans="2:2">
+      <c r="B166" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="167" spans="2:2">
+      <c r="B167" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="168" spans="2:2">
+      <c r="B168" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="169" spans="2:2">
+      <c r="B169" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="170" spans="2:2">
+      <c r="B170" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="171" spans="2:2">
+      <c r="B171" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="172" spans="2:2">
+      <c r="B172" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="173" spans="2:2">
+      <c r="B173" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="174" spans="2:2">
+      <c r="B174" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="175" spans="2:2">
+      <c r="B175" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="176" spans="2:2">
+      <c r="B176" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="177" spans="2:2">
+      <c r="B177" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="178" spans="2:2">
+      <c r="B178" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="179" spans="2:2">
+      <c r="B179" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="180" spans="2:2">
+      <c r="B180" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="181" spans="2:2">
+      <c r="B181" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="182" spans="2:2">
+      <c r="B182" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="183" spans="2:2">
+      <c r="B183" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="184" spans="2:2">
+      <c r="B184" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="185" spans="2:2">
+      <c r="B185" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="186" spans="2:2">
+      <c r="B186" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="187" spans="2:2">
+      <c r="B187" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="188" spans="2:2">
+      <c r="B188" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="189" spans="2:2">
+      <c r="B189" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="190" spans="2:2">
+      <c r="B190" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="191" spans="2:2">
+      <c r="B191" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="192" spans="2:2">
+      <c r="B192" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="193" spans="2:2">
+      <c r="B193" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="196" spans="2:2" ht="23.25">
+      <c r="B196" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="197" spans="2:2">
+      <c r="B197" s="16"/>
+    </row>
+    <row r="198" spans="2:2">
+      <c r="B198" s="16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="199" spans="2:2">
+      <c r="B199" s="16"/>
+    </row>
+    <row r="200" spans="2:2">
+      <c r="B200" s="16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="201" spans="2:2">
+      <c r="B201" s="5"/>
+    </row>
+    <row r="202" spans="2:2">
+      <c r="B202" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="203" spans="2:2">
+      <c r="B203" s="16"/>
+    </row>
+    <row r="204" spans="2:2">
+      <c r="B204" s="18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="205" spans="2:2">
+      <c r="B205" s="16"/>
+    </row>
+    <row r="206" spans="2:2">
+      <c r="B206" s="18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="208" spans="2:2" ht="45">
+      <c r="B208" s="19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="210" spans="2:2" ht="23.25">
+      <c r="B210" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="211" spans="2:2">
+      <c r="B211" s="16"/>
+    </row>
+    <row r="212" spans="2:2">
+      <c r="B212" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="213" spans="2:2">
+      <c r="B213" s="16"/>
+    </row>
+    <row r="214" spans="2:2">
+      <c r="B214" s="16" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="215" spans="2:2">
+      <c r="B215" s="16"/>
+    </row>
+    <row r="216" spans="2:2">
+      <c r="B216" s="16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="218" spans="2:2" ht="30">
+      <c r="B218" s="14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="220" spans="2:2">
+      <c r="B220" s="20" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="221" spans="2:2">
+      <c r="B221" s="20" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="222" spans="2:2">
+      <c r="B222" s="20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="223" spans="2:2">
+      <c r="B223" s="20" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="225" spans="2:2">
+      <c r="B225" s="21" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="226" spans="2:2">
+      <c r="B226" s="22" t="s">
+        <v>233</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B204" r:id="rId1" display="http://localhost:8080/"/>
+    <hyperlink ref="B206" r:id="rId2" display="http://localhost:8081/"/>
+    <hyperlink ref="B226" r:id="rId3"/>
+    <hyperlink ref="B225" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>